<commit_message>
feat: get dropdown working activities and outcomes sheet
</commit_message>
<xml_diff>
--- a/chpl/chpl-service/annual.xlsx
+++ b/chpl/chpl-service/annual.xlsx
@@ -3,20 +3,84 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Report Information" r:id="rId3" sheetId="1"/>
-    <sheet name="Activities and Outcomes" r:id="rId4" sheetId="2"/>
-    <sheet name="Complaints" r:id="rId5" sheetId="3"/>
-    <sheet name="Surveillance Summary" r:id="rId6" sheetId="4"/>
-    <sheet name="Surveillance Experience" r:id="rId7" sheetId="5"/>
+    <sheet name="Lists" r:id="rId3" sheetId="1" state="hidden"/>
+    <sheet name="Report Information" r:id="rId4" sheetId="2"/>
+    <sheet name="Activities and Outcomes" r:id="rId5" sheetId="3"/>
+    <sheet name="Complaints" r:id="rId6" sheetId="4"/>
+    <sheet name="Surveillance Summary" r:id="rId7" sheetId="5"/>
+    <sheet name="Surveillance Experience" r:id="rId8" sheetId="6"/>
   </sheets>
+  <definedNames>
+    <definedName name="SurveillanceOutcomeList">Lists!$A$1:$A$8</definedName>
+    <definedName name="ProcessTypeList">Lists!$B$1:$B$5</definedName>
+    <definedName name="StatusList">Lists!$C$1:$C$4</definedName>
+    <definedName name="BooleanList">Lists!$D$1:$D$2</definedName>
+  </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="117">
+  <si>
+    <t>No non-conformity</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Resolved through corrective action</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Corrective action ongoing</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Certification suspended</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Certification withdrawn</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Surveillance in process</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Under investigation/review</t>
+  </si>
+  <si>
+    <t>Non-conformity substantiated - Unresolved - Other - [Please describe]</t>
+  </si>
+  <si>
+    <t>In-the-Field</t>
+  </si>
+  <si>
+    <t>Correspondence with Complainant/Developer</t>
+  </si>
+  <si>
+    <t>Controlled/Test Environment</t>
+  </si>
+  <si>
+    <t>Review of Websites/Written Documentation</t>
+  </si>
+  <si>
+    <t>Other - [Please describe]</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Withdrawn by ONC-ACB</t>
+  </si>
+  <si>
+    <t>Withdrawn by Developer</t>
+  </si>
+  <si>
+    <t>Withdrawn by Developer Under Surveillance/Review</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
   <si>
     <t>ONC-Authorized Certification Body (ONC-ACB) 2019 Report Template for Surveillance Results</t>
   </si>
@@ -454,18 +518,6 @@
     <t>Primary Surveillance Processes</t>
   </si>
   <si>
-    <t>In-the-Field</t>
-  </si>
-  <si>
-    <t>Controlled/Test Environment</t>
-  </si>
-  <si>
-    <t>Correspondence with Complainant/Developer</t>
-  </si>
-  <si>
-    <t>Review of Websites/Written Documentation</t>
-  </si>
-  <si>
     <t>Other</t>
   </si>
   <si>
@@ -544,13 +596,44 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="25">
+  <fonts count="31">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <b val="true"/>
+      <i val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <i val="true"/>
+      <u val="single"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2013,7 +2096,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -2039,54 +2122,6 @@
       <alignment vertical="bottom" horizontal="left" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="top" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="35" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="41" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="46" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="top" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="51" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
@@ -2111,39 +2146,51 @@
       <alignment vertical="bottom" horizontal="left" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="65" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="top" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="69" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="73" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="35" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="77" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="41" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="81" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="46" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="top" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="51" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="56" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -2172,50 +2219,38 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="88" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="65" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="93" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="100" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="105" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="69" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="111" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="73" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="117" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="77" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="122" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="127" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="132" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="81" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -2243,11 +2278,83 @@
       <alignment vertical="bottom" horizontal="left" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="14" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="88" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="93" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="100" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="105" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="25" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="right" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="111" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="117" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="122" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="127" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="132" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="top" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="bottom" horizontal="left" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="left" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="8" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="top" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -2257,12 +2364,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="16384" hidden="true" width="8.0" customWidth="false"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="8DB4E2"/>
   </sheetPr>
   <dimension ref="A2:D54"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true" showGridLines="false" showRowColHeaders="false"/>
+    <sheetView workbookViewId="0" showGridLines="false" showRowColHeaders="false"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
@@ -2273,222 +2469,222 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
+      <c r="B2" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="7" t="s">
-        <v>1</v>
+      <c r="B3" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="3" t="s">
-        <v>2</v>
+      <c r="B5" s="15" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" ht="60.0" customHeight="true">
-      <c r="B6" s="4" t="s">
-        <v>3</v>
+      <c r="B6" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
+      <c r="A8" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9">
-      <c r="B9" s="2" t="s">
-        <v>6</v>
+      <c r="B9" s="14" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="10">
-      <c r="B10" s="13" t="s">
-        <v>7</v>
+      <c r="B10" s="25" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>9</v>
+      <c r="A12" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13">
-      <c r="B13" s="2" t="s">
-        <v>10</v>
+      <c r="B13" s="14" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="13" t="s">
-        <v>11</v>
+      <c r="B14" s="25" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>13</v>
+      <c r="A16" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="17" ht="30.0" customHeight="true">
-      <c r="B17" s="4" t="s">
-        <v>14</v>
+      <c r="B17" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" ht="120.0" customHeight="true">
-      <c r="B18" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
+      <c r="B18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="20">
-      <c r="B20" s="2" t="s">
-        <v>16</v>
+      <c r="B20" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>18</v>
+      <c r="A22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="8" t="s">
-        <v>19</v>
+      <c r="B23" s="20" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24">
-      <c r="B24" s="2" t="s">
-        <v>20</v>
+      <c r="B24" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>22</v>
+      <c r="B26" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="27" ht="30.0" customHeight="true">
-      <c r="B27" s="17"/>
-      <c r="C27" s="19"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="31"/>
     </row>
     <row r="28" ht="30.0" customHeight="true">
-      <c r="B28" s="17"/>
-      <c r="C28" s="19"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="31"/>
     </row>
     <row r="29" ht="30.0" customHeight="true">
-      <c r="B29" s="17"/>
-      <c r="C29" s="19"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="31"/>
     </row>
     <row r="30" ht="30.0" customHeight="true">
-      <c r="B30" s="17"/>
-      <c r="C30" s="19"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="31"/>
     </row>
     <row r="31" ht="30.0" customHeight="true">
-      <c r="B31" s="17"/>
-      <c r="C31" s="19"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="31"/>
     </row>
     <row r="32" ht="30.0" customHeight="true">
-      <c r="B32" s="17"/>
-      <c r="C32" s="19"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="31"/>
     </row>
     <row r="33" ht="30.0" customHeight="true">
-      <c r="B33" s="17"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="31"/>
     </row>
     <row r="34" ht="30.0" customHeight="true">
-      <c r="B34" s="17"/>
-      <c r="C34" s="19"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="31"/>
     </row>
     <row r="35" ht="30.0" customHeight="true">
-      <c r="B35" s="17"/>
-      <c r="C35" s="19"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="31"/>
     </row>
     <row r="36" ht="30.0" customHeight="true">
-      <c r="B36" s="20"/>
-      <c r="C36" s="21"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="33"/>
     </row>
     <row r="38">
-      <c r="B38" s="8" t="s">
-        <v>23</v>
+      <c r="B38" s="20" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="39" ht="45.0" customHeight="true">
-      <c r="B39" s="4" t="s">
-        <v>24</v>
+      <c r="B39" s="16" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="40" ht="60.0" customHeight="true">
-      <c r="B40" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="B40" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="D40" s="36"/>
     </row>
     <row r="42">
-      <c r="A42" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>27</v>
+      <c r="A42" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="43">
-      <c r="B43" s="8" t="s">
-        <v>28</v>
+      <c r="B43" s="20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="44" ht="30.0" customHeight="true">
-      <c r="B44" s="4" t="s">
-        <v>29</v>
+      <c r="B44" s="16" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="46" ht="60.0" customHeight="true">
-      <c r="B46" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="23"/>
-      <c r="D46" s="24"/>
+      <c r="B46" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="35"/>
+      <c r="D46" s="36"/>
     </row>
     <row r="48">
-      <c r="B48" s="8" t="s">
-        <v>31</v>
+      <c r="B48" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="49" ht="30.0" customHeight="true">
-      <c r="B49" s="4" t="s">
-        <v>32</v>
+      <c r="B49" s="16" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="51" ht="60.0" customHeight="true">
-      <c r="B51" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="24"/>
+      <c r="B51" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="35"/>
+      <c r="D51" s="36"/>
     </row>
     <row r="53">
-      <c r="A53" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>35</v>
+      <c r="A53" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="2" t="s">
-        <v>36</v>
+      <c r="B54" s="14" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2511,7 +2707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="8DB4E2"/>
@@ -2558,379 +2754,396 @@
   </cols>
   <sheetData>
     <row r="2" ht="90.0" customHeight="true">
-      <c r="B2" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="O2" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="P2" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" s="38" t="s">
+      <c r="B2" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="38" t="s">
+      <c r="C2" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="38" t="s">
+      <c r="D2" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="38" t="s">
+      <c r="E2" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="38" t="s">
+      <c r="F2" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="38" t="s">
+      <c r="G2" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="38" t="s">
+      <c r="H2" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="AB2" s="38" t="s">
+      <c r="I2" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="38" t="s">
+      <c r="J2" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" s="38" t="s">
+      <c r="K2" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="AE2" s="38" t="s">
+      <c r="L2" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="AF2" s="38" t="s">
+      <c r="M2" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="AG2" s="38" t="s">
+      <c r="N2" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="AH2" s="40"/>
-      <c r="AI2" s="41"/>
+      <c r="O2" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="50" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="T2" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="W2" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="X2" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y2" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z2" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA2" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC2" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD2" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE2" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF2" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG2" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="52"/>
+      <c r="AI2" s="53"/>
     </row>
     <row r="3">
-      <c r="B3" s="39"/>
-      <c r="AI3" s="42"/>
+      <c r="B3" s="51"/>
+      <c r="AI3" s="54"/>
     </row>
     <row r="4">
-      <c r="B4" s="39"/>
-      <c r="AI4" s="42"/>
+      <c r="B4" s="51"/>
+      <c r="AI4" s="54"/>
     </row>
     <row r="5">
-      <c r="B5" s="39"/>
-      <c r="AI5" s="42"/>
+      <c r="B5" s="51"/>
+      <c r="AI5" s="54"/>
     </row>
     <row r="6">
-      <c r="B6" s="39"/>
-      <c r="AI6" s="42"/>
+      <c r="B6" s="51"/>
+      <c r="AI6" s="54"/>
     </row>
     <row r="7">
-      <c r="B7" s="39"/>
-      <c r="AI7" s="42"/>
+      <c r="B7" s="51"/>
+      <c r="AI7" s="54"/>
     </row>
     <row r="8">
-      <c r="B8" s="39"/>
-      <c r="AI8" s="42"/>
+      <c r="B8" s="51"/>
+      <c r="AI8" s="54"/>
     </row>
     <row r="9">
-      <c r="B9" s="39"/>
-      <c r="AI9" s="42"/>
+      <c r="B9" s="51"/>
+      <c r="AI9" s="54"/>
     </row>
     <row r="10">
-      <c r="B10" s="39"/>
-      <c r="AI10" s="42"/>
+      <c r="B10" s="51"/>
+      <c r="AI10" s="54"/>
     </row>
     <row r="11">
-      <c r="B11" s="39"/>
-      <c r="AI11" s="42"/>
+      <c r="B11" s="51"/>
+      <c r="AI11" s="54"/>
     </row>
     <row r="12">
-      <c r="B12" s="39"/>
-      <c r="AI12" s="42"/>
+      <c r="B12" s="51"/>
+      <c r="AI12" s="54"/>
     </row>
     <row r="13">
-      <c r="B13" s="39"/>
-      <c r="AI13" s="42"/>
+      <c r="B13" s="51"/>
+      <c r="AI13" s="54"/>
     </row>
     <row r="14">
-      <c r="B14" s="39"/>
-      <c r="AI14" s="42"/>
+      <c r="B14" s="51"/>
+      <c r="AI14" s="54"/>
     </row>
     <row r="15">
-      <c r="B15" s="39"/>
-      <c r="AI15" s="42"/>
+      <c r="B15" s="51"/>
+      <c r="AI15" s="54"/>
     </row>
     <row r="16">
-      <c r="B16" s="39"/>
-      <c r="AI16" s="42"/>
+      <c r="B16" s="51"/>
+      <c r="AI16" s="54"/>
     </row>
     <row r="17">
-      <c r="B17" s="39"/>
-      <c r="AI17" s="42"/>
+      <c r="B17" s="51"/>
+      <c r="AI17" s="54"/>
     </row>
     <row r="18">
-      <c r="B18" s="39"/>
-      <c r="AI18" s="42"/>
+      <c r="B18" s="51"/>
+      <c r="AI18" s="54"/>
     </row>
     <row r="19">
-      <c r="B19" s="39"/>
-      <c r="AI19" s="42"/>
+      <c r="B19" s="51"/>
+      <c r="AI19" s="54"/>
     </row>
     <row r="20">
-      <c r="B20" s="39"/>
-      <c r="AI20" s="42"/>
+      <c r="B20" s="51"/>
+      <c r="AI20" s="54"/>
     </row>
     <row r="21">
-      <c r="B21" s="39"/>
-      <c r="AI21" s="42"/>
+      <c r="B21" s="51"/>
+      <c r="AI21" s="54"/>
     </row>
     <row r="22">
-      <c r="B22" s="39"/>
-      <c r="AI22" s="42"/>
+      <c r="B22" s="51"/>
+      <c r="AI22" s="54"/>
     </row>
     <row r="23">
-      <c r="B23" s="39"/>
-      <c r="AI23" s="42"/>
+      <c r="B23" s="51"/>
+      <c r="AI23" s="54"/>
     </row>
     <row r="24">
-      <c r="B24" s="39"/>
-      <c r="AI24" s="42"/>
+      <c r="B24" s="51"/>
+      <c r="AI24" s="54"/>
     </row>
     <row r="25">
-      <c r="B25" s="39"/>
-      <c r="AI25" s="42"/>
+      <c r="B25" s="51"/>
+      <c r="AI25" s="54"/>
     </row>
     <row r="26">
-      <c r="B26" s="39"/>
-      <c r="AI26" s="42"/>
+      <c r="B26" s="51"/>
+      <c r="AI26" s="54"/>
     </row>
     <row r="27">
-      <c r="B27" s="39"/>
-      <c r="AI27" s="42"/>
+      <c r="B27" s="51"/>
+      <c r="AI27" s="54"/>
     </row>
     <row r="28">
-      <c r="B28" s="39"/>
-      <c r="AI28" s="42"/>
+      <c r="B28" s="51"/>
+      <c r="AI28" s="54"/>
     </row>
     <row r="29">
-      <c r="B29" s="39"/>
-      <c r="AI29" s="42"/>
+      <c r="B29" s="51"/>
+      <c r="AI29" s="54"/>
     </row>
     <row r="30">
-      <c r="B30" s="39"/>
-      <c r="AI30" s="42"/>
+      <c r="B30" s="51"/>
+      <c r="AI30" s="54"/>
     </row>
     <row r="31">
-      <c r="B31" s="39"/>
-      <c r="AI31" s="42"/>
+      <c r="B31" s="51"/>
+      <c r="AI31" s="54"/>
     </row>
     <row r="32">
-      <c r="B32" s="39"/>
-      <c r="AI32" s="42"/>
+      <c r="B32" s="51"/>
+      <c r="AI32" s="54"/>
     </row>
     <row r="33">
-      <c r="B33" s="39"/>
-      <c r="AI33" s="42"/>
+      <c r="B33" s="51"/>
+      <c r="AI33" s="54"/>
     </row>
     <row r="34">
-      <c r="B34" s="39"/>
-      <c r="AI34" s="42"/>
+      <c r="B34" s="51"/>
+      <c r="AI34" s="54"/>
     </row>
     <row r="35">
-      <c r="B35" s="39"/>
-      <c r="AI35" s="42"/>
+      <c r="B35" s="51"/>
+      <c r="AI35" s="54"/>
     </row>
     <row r="36">
-      <c r="B36" s="39"/>
-      <c r="AI36" s="42"/>
+      <c r="B36" s="51"/>
+      <c r="AI36" s="54"/>
     </row>
     <row r="37">
-      <c r="B37" s="39"/>
-      <c r="AI37" s="42"/>
+      <c r="B37" s="51"/>
+      <c r="AI37" s="54"/>
     </row>
     <row r="38">
-      <c r="B38" s="39"/>
-      <c r="AI38" s="42"/>
+      <c r="B38" s="51"/>
+      <c r="AI38" s="54"/>
     </row>
     <row r="39">
-      <c r="B39" s="39"/>
-      <c r="AI39" s="42"/>
+      <c r="B39" s="51"/>
+      <c r="AI39" s="54"/>
     </row>
     <row r="40">
-      <c r="B40" s="39"/>
-      <c r="AI40" s="42"/>
+      <c r="B40" s="51"/>
+      <c r="AI40" s="54"/>
     </row>
     <row r="41">
-      <c r="B41" s="39"/>
-      <c r="AI41" s="42"/>
+      <c r="B41" s="51"/>
+      <c r="AI41" s="54"/>
     </row>
     <row r="42">
-      <c r="B42" s="39"/>
-      <c r="AI42" s="42"/>
+      <c r="B42" s="51"/>
+      <c r="AI42" s="54"/>
     </row>
     <row r="43">
-      <c r="B43" s="39"/>
-      <c r="AI43" s="42"/>
+      <c r="B43" s="51"/>
+      <c r="AI43" s="54"/>
     </row>
     <row r="44">
-      <c r="B44" s="39"/>
-      <c r="AI44" s="42"/>
+      <c r="B44" s="51"/>
+      <c r="AI44" s="54"/>
     </row>
     <row r="45">
-      <c r="B45" s="39"/>
-      <c r="AI45" s="42"/>
+      <c r="B45" s="51"/>
+      <c r="AI45" s="54"/>
     </row>
     <row r="46">
-      <c r="B46" s="39"/>
-      <c r="AI46" s="42"/>
+      <c r="B46" s="51"/>
+      <c r="AI46" s="54"/>
     </row>
     <row r="47">
-      <c r="B47" s="39"/>
-      <c r="AI47" s="42"/>
+      <c r="B47" s="51"/>
+      <c r="AI47" s="54"/>
     </row>
     <row r="48">
-      <c r="B48" s="39"/>
-      <c r="AI48" s="42"/>
+      <c r="B48" s="51"/>
+      <c r="AI48" s="54"/>
     </row>
     <row r="49">
-      <c r="B49" s="39"/>
-      <c r="AI49" s="42"/>
+      <c r="B49" s="51"/>
+      <c r="AI49" s="54"/>
     </row>
     <row r="50">
-      <c r="B50" s="39"/>
-      <c r="AI50" s="42"/>
+      <c r="B50" s="51"/>
+      <c r="AI50" s="54"/>
     </row>
     <row r="51">
-      <c r="B51" s="39"/>
-      <c r="AI51" s="42"/>
+      <c r="B51" s="51"/>
+      <c r="AI51" s="54"/>
     </row>
     <row r="52">
-      <c r="B52" s="39"/>
-      <c r="AI52" s="42"/>
+      <c r="B52" s="51"/>
+      <c r="AI52" s="54"/>
     </row>
     <row r="53">
-      <c r="B53" s="39"/>
-      <c r="AI53" s="42"/>
+      <c r="B53" s="51"/>
+      <c r="AI53" s="54"/>
     </row>
     <row r="54">
-      <c r="B54" s="39"/>
-      <c r="AI54" s="42"/>
+      <c r="B54" s="51"/>
+      <c r="AI54" s="54"/>
     </row>
     <row r="55">
-      <c r="B55" s="39"/>
-      <c r="AI55" s="42"/>
+      <c r="B55" s="51"/>
+      <c r="AI55" s="54"/>
     </row>
     <row r="56">
-      <c r="B56" s="39"/>
-      <c r="AI56" s="42"/>
+      <c r="B56" s="51"/>
+      <c r="AI56" s="54"/>
     </row>
     <row r="57">
-      <c r="B57" s="39"/>
-      <c r="AI57" s="42"/>
+      <c r="B57" s="51"/>
+      <c r="AI57" s="54"/>
     </row>
     <row r="58">
-      <c r="B58" s="39"/>
-      <c r="AI58" s="42"/>
+      <c r="B58" s="51"/>
+      <c r="AI58" s="54"/>
     </row>
     <row r="59">
-      <c r="B59" s="39"/>
-      <c r="AI59" s="42"/>
+      <c r="B59" s="51"/>
+      <c r="AI59" s="54"/>
     </row>
     <row r="60">
-      <c r="B60" s="39"/>
-      <c r="AI60" s="42"/>
+      <c r="B60" s="51"/>
+      <c r="AI60" s="54"/>
     </row>
     <row r="61">
-      <c r="B61" s="43"/>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
-      <c r="K61" s="44"/>
-      <c r="L61" s="44"/>
-      <c r="M61" s="44"/>
-      <c r="N61" s="44"/>
-      <c r="O61" s="44"/>
-      <c r="P61" s="44"/>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="44"/>
-      <c r="S61" s="44"/>
-      <c r="T61" s="44"/>
-      <c r="U61" s="44"/>
-      <c r="V61" s="44"/>
-      <c r="W61" s="44"/>
-      <c r="X61" s="44"/>
-      <c r="Y61" s="44"/>
-      <c r="Z61" s="44"/>
-      <c r="AA61" s="44"/>
-      <c r="AB61" s="44"/>
-      <c r="AC61" s="44"/>
-      <c r="AD61" s="44"/>
-      <c r="AE61" s="44"/>
-      <c r="AF61" s="44"/>
-      <c r="AG61" s="44"/>
-      <c r="AH61" s="44"/>
-      <c r="AI61" s="45"/>
+      <c r="B61" s="55"/>
+      <c r="C61" s="56"/>
+      <c r="D61" s="56"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="56"/>
+      <c r="H61" s="56"/>
+      <c r="I61" s="56"/>
+      <c r="J61" s="56"/>
+      <c r="K61" s="56"/>
+      <c r="L61" s="56"/>
+      <c r="M61" s="56"/>
+      <c r="N61" s="56"/>
+      <c r="O61" s="56"/>
+      <c r="P61" s="56"/>
+      <c r="Q61" s="56"/>
+      <c r="R61" s="56"/>
+      <c r="S61" s="56"/>
+      <c r="T61" s="56"/>
+      <c r="U61" s="56"/>
+      <c r="V61" s="56"/>
+      <c r="W61" s="56"/>
+      <c r="X61" s="56"/>
+      <c r="Y61" s="56"/>
+      <c r="Z61" s="56"/>
+      <c r="AA61" s="56"/>
+      <c r="AB61" s="56"/>
+      <c r="AC61" s="56"/>
+      <c r="AD61" s="56"/>
+      <c r="AE61" s="56"/>
+      <c r="AF61" s="56"/>
+      <c r="AG61" s="56"/>
+      <c r="AH61" s="56"/>
+      <c r="AI61" s="57"/>
     </row>
   </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" sqref="N3:N61" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>BooleanList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="S3:S61" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>SurveillanceOutcomeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="U3:U61" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>StatusList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="W3:W61" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>ProcessTypeList</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="V3:V61" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>BooleanList</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2942,7 +3155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="C4D79B"/>
@@ -2962,284 +3175,284 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="64" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="64" t="s">
-        <v>72</v>
+      <c r="B2" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="76" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="70" t="s">
+        <v>88</v>
+      </c>
+      <c r="H2" s="76" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="65"/>
-      <c r="G3" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="65"/>
+      <c r="B3" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="77"/>
+      <c r="G3" s="71" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="77"/>
     </row>
     <row r="4">
-      <c r="B4" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D4" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E4" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G4" s="62" t="s">
-        <v>90</v>
-      </c>
-      <c r="H4" s="66" t="n">
+      <c r="B4" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D4" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E4" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G4" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="78" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="77"/>
+      <c r="G5" s="74" t="s">
+        <v>106</v>
+      </c>
+      <c r="H5" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D6" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E6" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G6" s="71" t="s">
+        <v>107</v>
+      </c>
+      <c r="H6" s="77"/>
+    </row>
+    <row r="7">
+      <c r="B7" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D7" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E7" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G7" s="74" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D8" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E8" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G8" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D9" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E9" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="H9" s="77"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D10" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E10" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="G10" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="H10" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="77"/>
+      <c r="G11" s="79" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" s="80" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D12" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E12" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D13" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E13" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D14" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E14" s="78" t="n">
+        <v>-1.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="65"/>
-      <c r="G5" s="62" t="s">
-        <v>91</v>
-      </c>
-      <c r="H5" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="62" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D6" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E6" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G6" s="59" t="s">
-        <v>92</v>
-      </c>
-      <c r="H6" s="65"/>
-    </row>
-    <row r="7">
-      <c r="B7" s="62" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D7" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E7" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G7" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D8" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E8" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G8" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="H8" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="62" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D9" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E9" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G9" s="59" t="s">
-        <v>95</v>
-      </c>
-      <c r="H9" s="65"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="62" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D10" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E10" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="G10" s="62" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="59" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="65"/>
-      <c r="G11" s="67" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="68" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" s="62" t="s">
-        <v>82</v>
-      </c>
-      <c r="C12" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D12" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E12" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D13" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E13" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D14" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E14" s="66" t="n">
-        <v>-1.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="65"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="77"/>
     </row>
     <row r="16">
-      <c r="B16" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="C16" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D16" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E16" s="66" t="n">
+      <c r="B16" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D16" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E16" s="78" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D17" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E17" s="66" t="n">
+      <c r="B17" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D17" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E17" s="78" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="62" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D18" s="63" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E18" s="66" t="n">
+      <c r="B18" s="74" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D18" s="75" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E18" s="78" t="n">
         <v>-1.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="69" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="D19" s="69" t="n">
-        <v>-1.0</v>
-      </c>
-      <c r="E19" s="68" t="n">
+      <c r="B19" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" s="81" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="D19" s="81" t="n">
+        <v>-1.0</v>
+      </c>
+      <c r="E19" s="80" t="n">
         <v>-1.0</v>
       </c>
     </row>
@@ -3248,7 +3461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="C4D79B"/>
@@ -3267,23 +3480,23 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="82" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="F2" s="82" t="s">
-        <v>100</v>
+      <c r="B2" s="94" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="F2" s="94" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" ht="315.0" customHeight="true">
-      <c r="B3" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="F3" s="83" t="s">
-        <v>101</v>
+      <c r="B3" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="F3" s="95" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>